<commit_message>
Fixes tests after removal of storage type
</commit_message>
<xml_diff>
--- a/inst/extdata/Banet-Example/metadata/enclosure-study-growth-rates-metadata.xlsx
+++ b/inst/extdata/Banet-Example/metadata/enclosure-study-growth-rates-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\EMLaide\inst\extdata\Banet-Example\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EMLaide\inst\extdata\Banet-Example\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889FFC07-DEF6-4C13-A5BE-E345E38F0880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB83BE4-A8F5-492A-BAD9-0E61DB03862D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10080" yWindow="-16560" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="138">
   <si>
     <t>first_name</t>
   </si>
@@ -206,9 +206,6 @@
     <t>project_title</t>
   </si>
   <si>
-    <t>storage_type</t>
-  </si>
-  <si>
     <t xml:space="preserve">organization </t>
   </si>
   <si>
@@ -318,12 +315,6 @@
   </si>
   <si>
     <t>steelhead</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>dbl</t>
   </si>
   <si>
     <t>nominal</t>
@@ -966,21 +957,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +992,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1006,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>30</v>
@@ -1047,12 +1038,12 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1068,3317 +1059,3098 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMH16384"/>
+  <dimension ref="A1:AMG16384"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="19.625" style="1"/>
-    <col min="3" max="3" width="13.125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="16" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.125" style="1" customWidth="1"/>
-    <col min="15" max="1022" width="19.625" style="1"/>
-    <col min="1023" max="1025" width="8.375" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.125" style="1" customWidth="1"/>
+    <col min="14" max="1021" width="19.625" style="1"/>
+    <col min="1022" max="1024" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>56</v>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>95</v>
+      <c r="C2" s="12" t="s">
+        <v>93</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>96</v>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
+        <v>94</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2"/>
       <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="14"/>
-    </row>
-    <row r="3" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="L2" s="15"/>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>95</v>
+      <c r="C3" s="12" t="s">
+        <v>93</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>96</v>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>94</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-    </row>
-    <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12">
+        <v>48</v>
+      </c>
+      <c r="M4" s="12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12">
+        <v>68</v>
+      </c>
+      <c r="M5" s="12">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12">
+        <v>65</v>
+      </c>
+      <c r="M6" s="12">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B7" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7">
+        <v>0.33500227580000003</v>
+      </c>
+      <c r="M7">
+        <v>2.7003188819999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8">
+        <v>0.73275677299999997</v>
+      </c>
+      <c r="M8">
+        <v>1.590976199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
-        <v>100</v>
+      <c r="I9" s="13"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12">
+        <v>18</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="M9" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>129</v>
+      <c r="I10" s="13"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12">
+        <v>11</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>99</v>
+      <c r="M10" s="12">
+        <v>20</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12">
-        <v>48</v>
+    </row>
+    <row r="11" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>108</v>
       </c>
-      <c r="N4" s="12">
-        <v>78</v>
+      <c r="B11" s="12" t="s">
+        <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
-        <v>100</v>
+      <c r="I11" s="13"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12">
+        <v>5</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>98</v>
+      <c r="M11" s="12">
+        <v>20</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>129</v>
+    </row>
+    <row r="12" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>109</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>99</v>
+      <c r="B12" s="12" t="s">
+        <v>127</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12">
-        <v>68</v>
-      </c>
-      <c r="N5" s="12">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>98</v>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>97</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12">
-        <v>65</v>
-      </c>
-      <c r="N6" s="12">
+      <c r="F12" s="12" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>107</v>
+      <c r="G12" s="12" t="s">
+        <v>132</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>121</v>
+      <c r="H12" s="12" t="s">
+        <v>96</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>95</v>
+      <c r="I12" s="13"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12">
+        <v>593.19299999999998</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>98</v>
+      <c r="M12" s="12">
+        <v>628.54999999999995</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7">
-        <v>0.33500227580000003</v>
-      </c>
-      <c r="N7">
-        <v>2.7003188819999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8">
-        <v>0.73275677299999997</v>
-      </c>
-      <c r="N8">
-        <v>1.590976199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12">
-        <v>18</v>
-      </c>
-      <c r="N9" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="13" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>95</v>
+      <c r="C13" s="12" t="s">
+        <v>93</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12">
-        <v>11</v>
-      </c>
-      <c r="N10" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12">
-        <v>5</v>
-      </c>
-      <c r="N11" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12">
-        <v>593.19299999999998</v>
-      </c>
-      <c r="N12" s="12">
-        <v>628.54999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-    </row>
-    <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="J15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="12"/>
       <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12">
+      <c r="L15" s="12">
         <v>43</v>
       </c>
-      <c r="N15" s="12">
+      <c r="M15" s="12">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="13"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="12"/>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34" s="12"/>
-      <c r="C34" s="13"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="12"/>
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="13"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="12"/>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36" s="12"/>
-      <c r="C36" s="13"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="13"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="13"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="12"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39" s="12"/>
-      <c r="C39" s="13"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="12"/>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" s="12"/>
-      <c r="C40" s="13"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="12"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41" s="12"/>
-      <c r="C41" s="13"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
       <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42" s="12"/>
-      <c r="C42" s="13"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="12"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43" s="12"/>
-      <c r="C43" s="13"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44" s="12"/>
-      <c r="C44" s="13"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="12"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45" s="12"/>
-      <c r="C45" s="13"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="12"/>
       <c r="K45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46" s="12"/>
-      <c r="C46" s="13"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="12"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47" s="12"/>
-      <c r="C47" s="13"/>
+      <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="12"/>
       <c r="K47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48" s="12"/>
-      <c r="C48" s="13"/>
+      <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49" s="12"/>
-      <c r="C49" s="13"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="12"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50" s="12"/>
-      <c r="C50" s="13"/>
+      <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="12"/>
       <c r="K50" s="12"/>
       <c r="L50" s="12"/>
       <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51" s="12"/>
-      <c r="C51" s="13"/>
+      <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="12"/>
       <c r="K51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52" s="12"/>
-      <c r="C52" s="13"/>
+      <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
       <c r="G52" s="12"/>
       <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="12"/>
       <c r="K52" s="12"/>
       <c r="L52" s="12"/>
       <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53" s="12"/>
-      <c r="C53" s="13"/>
+      <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
       <c r="G53" s="12"/>
       <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
       <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54" s="12"/>
-      <c r="C54" s="13"/>
+      <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
       <c r="G54" s="12"/>
       <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="12"/>
       <c r="K54" s="12"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55" s="12"/>
-      <c r="C55" s="13"/>
+      <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
       <c r="F55" s="12"/>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="12"/>
       <c r="K55" s="12"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56" s="12"/>
-      <c r="C56" s="13"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="12"/>
       <c r="K56" s="12"/>
       <c r="L56" s="12"/>
       <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57" s="12"/>
-      <c r="C57" s="13"/>
+      <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="12"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58" s="12"/>
-      <c r="C58" s="13"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
       <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="12"/>
       <c r="K58" s="12"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59" s="12"/>
-      <c r="C59" s="13"/>
+      <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
       <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="12"/>
       <c r="K59" s="12"/>
       <c r="L59" s="12"/>
       <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60" s="12"/>
-      <c r="C60" s="13"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="12"/>
       <c r="K60" s="12"/>
       <c r="L60" s="12"/>
       <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61" s="12"/>
-      <c r="C61" s="13"/>
+      <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
       <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="12"/>
       <c r="K61" s="12"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62" s="12"/>
-      <c r="C62" s="13"/>
+      <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
       <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="12"/>
       <c r="K62" s="12"/>
       <c r="L62" s="12"/>
       <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63" s="12"/>
-      <c r="C63" s="13"/>
+      <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
       <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="12"/>
       <c r="K63" s="12"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64" s="12"/>
-      <c r="C64" s="13"/>
+      <c r="C64" s="12"/>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
       <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="12"/>
       <c r="K64" s="12"/>
       <c r="L64" s="12"/>
       <c r="M64" s="12"/>
-      <c r="N64" s="12"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65" s="12"/>
-      <c r="C65" s="13"/>
+      <c r="C65" s="12"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
       <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="12"/>
       <c r="K65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
-      <c r="N65" s="12"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66" s="12"/>
-      <c r="C66" s="13"/>
+      <c r="C66" s="12"/>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
       <c r="H66" s="12"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="12"/>
       <c r="K66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12"/>
-      <c r="N66" s="12"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67"/>
       <c r="B67" s="12"/>
-      <c r="C67" s="13"/>
+      <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="12"/>
       <c r="K67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12"/>
-      <c r="N67" s="12"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68" s="12"/>
-      <c r="C68" s="13"/>
+      <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
       <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="12"/>
       <c r="K68" s="12"/>
       <c r="L68" s="12"/>
       <c r="M68" s="12"/>
-      <c r="N68" s="12"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69"/>
       <c r="B69" s="12"/>
-      <c r="C69" s="13"/>
+      <c r="C69" s="12"/>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
       <c r="G69" s="12"/>
       <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="12"/>
       <c r="K69" s="12"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12"/>
-      <c r="N69" s="12"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70" s="12"/>
-      <c r="C70" s="13"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
       <c r="F70" s="12"/>
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="12"/>
       <c r="K70" s="12"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12"/>
-      <c r="N70" s="12"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71" s="12"/>
-      <c r="C71" s="13"/>
+      <c r="C71" s="12"/>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="12"/>
       <c r="K71" s="12"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72" s="12"/>
-      <c r="C72" s="13"/>
+      <c r="C72" s="12"/>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
       <c r="H72" s="12"/>
-      <c r="I72" s="12"/>
-      <c r="J72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="12"/>
       <c r="K72" s="12"/>
       <c r="L72" s="12"/>
       <c r="M72" s="12"/>
-      <c r="N72" s="12"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73"/>
       <c r="B73" s="12"/>
-      <c r="C73" s="13"/>
+      <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
       <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="12"/>
       <c r="K73" s="12"/>
       <c r="L73" s="12"/>
       <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74" s="12"/>
-      <c r="C74" s="13"/>
+      <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="12"/>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
       <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="12"/>
       <c r="K74" s="12"/>
       <c r="L74" s="12"/>
       <c r="M74" s="12"/>
-      <c r="N74" s="12"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75" s="12"/>
-      <c r="C75" s="13"/>
+      <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="12"/>
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
       <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="12"/>
       <c r="K75" s="12"/>
       <c r="L75" s="12"/>
       <c r="M75" s="12"/>
-      <c r="N75" s="12"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76" s="12"/>
-      <c r="C76" s="13"/>
+      <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
       <c r="F76" s="12"/>
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
-      <c r="J76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="12"/>
       <c r="K76" s="12"/>
       <c r="L76" s="12"/>
       <c r="M76" s="12"/>
-      <c r="N76" s="12"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77"/>
       <c r="B77" s="12"/>
-      <c r="C77" s="13"/>
+      <c r="C77" s="12"/>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
       <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="12"/>
       <c r="K77" s="12"/>
       <c r="L77" s="12"/>
       <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78" s="12"/>
-      <c r="C78" s="13"/>
+      <c r="C78" s="12"/>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="12"/>
       <c r="K78" s="12"/>
       <c r="L78" s="12"/>
       <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79"/>
       <c r="B79" s="12"/>
-      <c r="C79" s="13"/>
+      <c r="C79" s="12"/>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="12"/>
       <c r="K79" s="12"/>
       <c r="L79" s="12"/>
       <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80"/>
       <c r="B80" s="12"/>
-      <c r="C80" s="13"/>
+      <c r="C80" s="12"/>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="12"/>
       <c r="K80" s="12"/>
       <c r="L80" s="12"/>
       <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81"/>
       <c r="B81" s="12"/>
-      <c r="C81" s="13"/>
+      <c r="C81" s="12"/>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
       <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="12"/>
       <c r="K81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12"/>
-      <c r="N81" s="12"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82"/>
       <c r="B82" s="12"/>
-      <c r="C82" s="13"/>
+      <c r="C82" s="12"/>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
       <c r="F82" s="12"/>
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="12"/>
       <c r="K82" s="12"/>
       <c r="L82" s="12"/>
       <c r="M82" s="12"/>
-      <c r="N82" s="12"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83"/>
       <c r="B83" s="12"/>
-      <c r="C83" s="13"/>
+      <c r="C83" s="12"/>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="12"/>
       <c r="K83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
-      <c r="N83" s="12"/>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84"/>
       <c r="B84" s="12"/>
-      <c r="C84" s="13"/>
+      <c r="C84" s="12"/>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="12"/>
       <c r="K84" s="12"/>
       <c r="L84" s="12"/>
       <c r="M84" s="12"/>
-      <c r="N84" s="12"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85"/>
       <c r="B85" s="12"/>
-      <c r="C85" s="13"/>
+      <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
-      <c r="J85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="12"/>
       <c r="K85" s="12"/>
       <c r="L85" s="12"/>
       <c r="M85" s="12"/>
-      <c r="N85" s="12"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86"/>
       <c r="B86" s="12"/>
-      <c r="C86" s="13"/>
+      <c r="C86" s="12"/>
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
-      <c r="I86" s="12"/>
-      <c r="J86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="12"/>
       <c r="K86" s="12"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12"/>
-      <c r="N86" s="12"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87"/>
       <c r="B87" s="12"/>
-      <c r="C87" s="13"/>
+      <c r="C87" s="12"/>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="12"/>
-      <c r="J87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="12"/>
       <c r="K87" s="12"/>
       <c r="L87" s="12"/>
       <c r="M87" s="12"/>
-      <c r="N87" s="12"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88"/>
       <c r="B88" s="12"/>
-      <c r="C88" s="13"/>
+      <c r="C88" s="12"/>
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="12"/>
       <c r="K88" s="12"/>
       <c r="L88" s="12"/>
       <c r="M88" s="12"/>
-      <c r="N88" s="12"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89"/>
       <c r="B89" s="12"/>
-      <c r="C89" s="13"/>
+      <c r="C89" s="12"/>
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
       <c r="F89" s="12"/>
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
-      <c r="I89" s="12"/>
-      <c r="J89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="12"/>
       <c r="K89" s="12"/>
       <c r="L89" s="12"/>
       <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90"/>
       <c r="B90" s="12"/>
-      <c r="C90" s="13"/>
+      <c r="C90" s="12"/>
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
       <c r="F90" s="12"/>
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
-      <c r="I90" s="12"/>
-      <c r="J90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="12"/>
       <c r="K90" s="12"/>
       <c r="L90" s="12"/>
       <c r="M90" s="12"/>
-      <c r="N90" s="12"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91"/>
       <c r="B91" s="12"/>
-      <c r="C91" s="13"/>
+      <c r="C91" s="12"/>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
       <c r="F91" s="12"/>
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
-      <c r="I91" s="12"/>
-      <c r="J91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="12"/>
       <c r="K91" s="12"/>
       <c r="L91" s="12"/>
       <c r="M91" s="12"/>
-      <c r="N91" s="12"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92"/>
       <c r="B92" s="12"/>
-      <c r="C92" s="13"/>
+      <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
-      <c r="I92" s="12"/>
-      <c r="J92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="12"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
       <c r="M92" s="12"/>
-      <c r="N92" s="12"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93"/>
       <c r="B93" s="12"/>
-      <c r="C93" s="13"/>
+      <c r="C93" s="12"/>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
       <c r="F93" s="12"/>
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
-      <c r="I93" s="12"/>
-      <c r="J93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="12"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
       <c r="M93" s="12"/>
-      <c r="N93" s="12"/>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94"/>
       <c r="B94" s="12"/>
-      <c r="C94" s="13"/>
+      <c r="C94" s="12"/>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
       <c r="F94" s="12"/>
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
-      <c r="I94" s="12"/>
-      <c r="J94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="12"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="12"/>
-      <c r="N94" s="12"/>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95"/>
       <c r="B95" s="12"/>
-      <c r="C95" s="13"/>
+      <c r="C95" s="12"/>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
       <c r="F95" s="12"/>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
-      <c r="I95" s="12"/>
-      <c r="J95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="12"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
-      <c r="N95" s="12"/>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96"/>
       <c r="B96" s="12"/>
-      <c r="C96" s="13"/>
+      <c r="C96" s="12"/>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
       <c r="F96" s="12"/>
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
-      <c r="I96" s="12"/>
-      <c r="J96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="12"/>
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
       <c r="M96" s="12"/>
-      <c r="N96" s="12"/>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97" s="12"/>
-      <c r="C97" s="13"/>
+      <c r="C97" s="12"/>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
       <c r="F97" s="12"/>
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
-      <c r="I97" s="12"/>
-      <c r="J97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="12"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
       <c r="M97" s="12"/>
-      <c r="N97" s="12"/>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98"/>
       <c r="B98" s="12"/>
-      <c r="C98" s="13"/>
+      <c r="C98" s="12"/>
       <c r="D98" s="12"/>
       <c r="E98" s="12"/>
       <c r="F98" s="12"/>
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
-      <c r="I98" s="12"/>
-      <c r="J98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="12"/>
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
       <c r="M98" s="12"/>
-      <c r="N98" s="12"/>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99"/>
       <c r="B99" s="12"/>
-      <c r="C99" s="13"/>
+      <c r="C99" s="12"/>
       <c r="D99" s="12"/>
       <c r="E99" s="12"/>
       <c r="F99" s="12"/>
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
-      <c r="I99" s="12"/>
-      <c r="J99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="12"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12"/>
-      <c r="N99" s="12"/>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100"/>
       <c r="B100" s="12"/>
-      <c r="C100" s="13"/>
+      <c r="C100" s="12"/>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="12"/>
       <c r="K100" s="12"/>
       <c r="L100" s="12"/>
       <c r="M100" s="12"/>
-      <c r="N100" s="12"/>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101"/>
       <c r="B101" s="12"/>
-      <c r="C101" s="13"/>
+      <c r="C101" s="12"/>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
-      <c r="I101" s="12"/>
-      <c r="J101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="12"/>
       <c r="K101" s="12"/>
       <c r="L101" s="12"/>
       <c r="M101" s="12"/>
-      <c r="N101" s="12"/>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102"/>
       <c r="B102" s="12"/>
-      <c r="C102" s="13"/>
+      <c r="C102" s="12"/>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
-      <c r="I102" s="12"/>
-      <c r="J102" s="13"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="12"/>
       <c r="K102" s="12"/>
       <c r="L102" s="12"/>
       <c r="M102" s="12"/>
-      <c r="N102" s="12"/>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103"/>
       <c r="B103" s="12"/>
-      <c r="C103" s="13"/>
+      <c r="C103" s="12"/>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
       <c r="F103" s="12"/>
       <c r="G103" s="12"/>
       <c r="H103" s="12"/>
-      <c r="I103" s="12"/>
-      <c r="J103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="12"/>
       <c r="K103" s="12"/>
       <c r="L103" s="12"/>
       <c r="M103" s="12"/>
-      <c r="N103" s="12"/>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104"/>
       <c r="B104" s="12"/>
-      <c r="C104" s="13"/>
+      <c r="C104" s="12"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
       <c r="F104" s="12"/>
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
-      <c r="I104" s="12"/>
-      <c r="J104" s="13"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="12"/>
       <c r="K104" s="12"/>
       <c r="L104" s="12"/>
       <c r="M104" s="12"/>
-      <c r="N104" s="12"/>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105"/>
       <c r="B105" s="12"/>
-      <c r="C105" s="13"/>
+      <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
       <c r="F105" s="12"/>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
-      <c r="I105" s="12"/>
-      <c r="J105" s="13"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="12"/>
       <c r="K105" s="12"/>
       <c r="L105" s="12"/>
       <c r="M105" s="12"/>
-      <c r="N105" s="12"/>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106"/>
       <c r="B106" s="12"/>
-      <c r="C106" s="13"/>
+      <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
-      <c r="I106" s="12"/>
-      <c r="J106" s="13"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="12"/>
       <c r="K106" s="12"/>
       <c r="L106" s="12"/>
       <c r="M106" s="12"/>
-      <c r="N106" s="12"/>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107"/>
       <c r="B107" s="12"/>
-      <c r="C107" s="13"/>
+      <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
       <c r="F107" s="12"/>
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
-      <c r="I107" s="12"/>
-      <c r="J107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="12"/>
       <c r="K107" s="12"/>
       <c r="L107" s="12"/>
       <c r="M107" s="12"/>
-      <c r="N107" s="12"/>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108"/>
       <c r="B108" s="12"/>
-      <c r="C108" s="13"/>
+      <c r="C108" s="12"/>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
       <c r="F108" s="12"/>
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
-      <c r="I108" s="12"/>
-      <c r="J108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="12"/>
       <c r="K108" s="12"/>
       <c r="L108" s="12"/>
       <c r="M108" s="12"/>
-      <c r="N108" s="12"/>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109"/>
       <c r="B109" s="12"/>
-      <c r="C109" s="13"/>
+      <c r="C109" s="12"/>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
       <c r="F109" s="12"/>
       <c r="G109" s="12"/>
       <c r="H109" s="12"/>
-      <c r="I109" s="12"/>
-      <c r="J109" s="13"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="12"/>
       <c r="K109" s="12"/>
       <c r="L109" s="12"/>
       <c r="M109" s="12"/>
-      <c r="N109" s="12"/>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110"/>
       <c r="B110" s="12"/>
-      <c r="C110" s="13"/>
+      <c r="C110" s="12"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
       <c r="F110" s="12"/>
       <c r="G110" s="12"/>
       <c r="H110" s="12"/>
-      <c r="I110" s="12"/>
-      <c r="J110" s="13"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="12"/>
       <c r="K110" s="12"/>
       <c r="L110" s="12"/>
       <c r="M110" s="12"/>
-      <c r="N110" s="12"/>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111"/>
       <c r="B111" s="12"/>
-      <c r="C111" s="13"/>
+      <c r="C111" s="12"/>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
       <c r="F111" s="12"/>
       <c r="G111" s="12"/>
       <c r="H111" s="12"/>
-      <c r="I111" s="12"/>
-      <c r="J111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="12"/>
       <c r="K111" s="12"/>
       <c r="L111" s="12"/>
       <c r="M111" s="12"/>
-      <c r="N111" s="12"/>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112"/>
       <c r="B112" s="12"/>
-      <c r="C112" s="13"/>
+      <c r="C112" s="12"/>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>
       <c r="F112" s="12"/>
       <c r="G112" s="12"/>
       <c r="H112" s="12"/>
-      <c r="I112" s="12"/>
-      <c r="J112" s="13"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="12"/>
       <c r="K112" s="12"/>
       <c r="L112" s="12"/>
       <c r="M112" s="12"/>
-      <c r="N112" s="12"/>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113"/>
       <c r="B113" s="12"/>
-      <c r="C113" s="13"/>
+      <c r="C113" s="12"/>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
       <c r="F113" s="12"/>
       <c r="G113" s="12"/>
       <c r="H113" s="12"/>
-      <c r="I113" s="12"/>
-      <c r="J113" s="13"/>
+      <c r="I113" s="13"/>
+      <c r="J113" s="12"/>
       <c r="K113" s="12"/>
       <c r="L113" s="12"/>
       <c r="M113" s="12"/>
-      <c r="N113" s="12"/>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114"/>
       <c r="B114" s="12"/>
-      <c r="C114" s="13"/>
+      <c r="C114" s="12"/>
       <c r="D114" s="12"/>
       <c r="E114" s="12"/>
       <c r="F114" s="12"/>
       <c r="G114" s="12"/>
       <c r="H114" s="12"/>
-      <c r="I114" s="12"/>
-      <c r="J114" s="13"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="12"/>
       <c r="K114" s="12"/>
       <c r="L114" s="12"/>
       <c r="M114" s="12"/>
-      <c r="N114" s="12"/>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115"/>
       <c r="B115" s="12"/>
-      <c r="C115" s="13"/>
+      <c r="C115" s="12"/>
       <c r="D115" s="12"/>
       <c r="E115" s="12"/>
       <c r="F115" s="12"/>
       <c r="G115" s="12"/>
       <c r="H115" s="12"/>
-      <c r="I115" s="12"/>
-      <c r="J115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="12"/>
       <c r="K115" s="12"/>
       <c r="L115" s="12"/>
       <c r="M115" s="12"/>
-      <c r="N115" s="12"/>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116"/>
       <c r="B116" s="12"/>
-      <c r="C116" s="13"/>
+      <c r="C116" s="12"/>
       <c r="D116" s="12"/>
       <c r="E116" s="12"/>
       <c r="F116" s="12"/>
       <c r="G116" s="12"/>
       <c r="H116" s="12"/>
-      <c r="I116" s="12"/>
-      <c r="J116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="12"/>
       <c r="K116" s="12"/>
       <c r="L116" s="12"/>
       <c r="M116" s="12"/>
-      <c r="N116" s="12"/>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117"/>
       <c r="B117" s="12"/>
-      <c r="C117" s="13"/>
+      <c r="C117" s="12"/>
       <c r="D117" s="12"/>
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
       <c r="G117" s="12"/>
       <c r="H117" s="12"/>
-      <c r="I117" s="12"/>
-      <c r="J117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="12"/>
       <c r="K117" s="12"/>
       <c r="L117" s="12"/>
       <c r="M117" s="12"/>
-      <c r="N117" s="12"/>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118"/>
       <c r="B118" s="12"/>
-      <c r="C118" s="13"/>
+      <c r="C118" s="12"/>
       <c r="D118" s="12"/>
       <c r="E118" s="12"/>
       <c r="F118" s="12"/>
       <c r="G118" s="12"/>
       <c r="H118" s="12"/>
-      <c r="I118" s="12"/>
-      <c r="J118" s="13"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="12"/>
       <c r="K118" s="12"/>
       <c r="L118" s="12"/>
       <c r="M118" s="12"/>
-      <c r="N118" s="12"/>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119"/>
       <c r="B119" s="12"/>
-      <c r="C119" s="13"/>
+      <c r="C119" s="12"/>
       <c r="D119" s="12"/>
       <c r="E119" s="12"/>
       <c r="F119" s="12"/>
       <c r="G119" s="12"/>
       <c r="H119" s="12"/>
-      <c r="I119" s="12"/>
-      <c r="J119" s="13"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="12"/>
       <c r="K119" s="12"/>
       <c r="L119" s="12"/>
       <c r="M119" s="12"/>
-      <c r="N119" s="12"/>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120"/>
       <c r="B120" s="12"/>
-      <c r="C120" s="13"/>
+      <c r="C120" s="12"/>
       <c r="D120" s="12"/>
       <c r="E120" s="12"/>
       <c r="F120" s="12"/>
       <c r="G120" s="12"/>
       <c r="H120" s="12"/>
-      <c r="I120" s="12"/>
-      <c r="J120" s="13"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="12"/>
       <c r="K120" s="12"/>
       <c r="L120" s="12"/>
       <c r="M120" s="12"/>
-      <c r="N120" s="12"/>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121"/>
       <c r="B121" s="12"/>
-      <c r="C121" s="13"/>
+      <c r="C121" s="12"/>
       <c r="D121" s="12"/>
       <c r="E121" s="12"/>
       <c r="F121" s="12"/>
       <c r="G121" s="12"/>
       <c r="H121" s="12"/>
-      <c r="I121" s="12"/>
-      <c r="J121" s="13"/>
+      <c r="I121" s="13"/>
+      <c r="J121" s="12"/>
       <c r="K121" s="12"/>
       <c r="L121" s="12"/>
       <c r="M121" s="12"/>
-      <c r="N121" s="12"/>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122"/>
       <c r="B122" s="12"/>
-      <c r="C122" s="13"/>
+      <c r="C122" s="12"/>
       <c r="D122" s="12"/>
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
       <c r="G122" s="12"/>
       <c r="H122" s="12"/>
-      <c r="I122" s="12"/>
-      <c r="J122" s="13"/>
+      <c r="I122" s="13"/>
+      <c r="J122" s="12"/>
       <c r="K122" s="12"/>
       <c r="L122" s="12"/>
       <c r="M122" s="12"/>
-      <c r="N122" s="12"/>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123"/>
       <c r="B123" s="12"/>
-      <c r="C123" s="13"/>
+      <c r="C123" s="12"/>
       <c r="D123" s="12"/>
       <c r="E123" s="12"/>
       <c r="F123" s="12"/>
       <c r="G123" s="12"/>
       <c r="H123" s="12"/>
-      <c r="I123" s="12"/>
-      <c r="J123" s="13"/>
+      <c r="I123" s="13"/>
+      <c r="J123" s="12"/>
       <c r="K123" s="12"/>
       <c r="L123" s="12"/>
       <c r="M123" s="12"/>
-      <c r="N123" s="12"/>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124"/>
       <c r="B124" s="12"/>
-      <c r="C124" s="13"/>
+      <c r="C124" s="12"/>
       <c r="D124" s="12"/>
       <c r="E124" s="12"/>
       <c r="F124" s="12"/>
       <c r="G124" s="12"/>
       <c r="H124" s="12"/>
-      <c r="I124" s="12"/>
-      <c r="J124" s="13"/>
+      <c r="I124" s="13"/>
+      <c r="J124" s="12"/>
       <c r="K124" s="12"/>
       <c r="L124" s="12"/>
       <c r="M124" s="12"/>
-      <c r="N124" s="12"/>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125"/>
       <c r="B125" s="12"/>
-      <c r="C125" s="13"/>
+      <c r="C125" s="12"/>
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
       <c r="F125" s="12"/>
       <c r="G125" s="12"/>
       <c r="H125" s="12"/>
-      <c r="I125" s="12"/>
-      <c r="J125" s="13"/>
+      <c r="I125" s="13"/>
+      <c r="J125" s="12"/>
       <c r="K125" s="12"/>
       <c r="L125" s="12"/>
       <c r="M125" s="12"/>
-      <c r="N125" s="12"/>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126"/>
       <c r="B126" s="12"/>
-      <c r="C126" s="13"/>
+      <c r="C126" s="12"/>
       <c r="D126" s="12"/>
       <c r="E126" s="12"/>
       <c r="F126" s="12"/>
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
-      <c r="I126" s="12"/>
-      <c r="J126" s="13"/>
+      <c r="I126" s="13"/>
+      <c r="J126" s="12"/>
       <c r="K126" s="12"/>
       <c r="L126" s="12"/>
       <c r="M126" s="12"/>
-      <c r="N126" s="12"/>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127"/>
       <c r="B127" s="12"/>
-      <c r="C127" s="13"/>
+      <c r="C127" s="12"/>
       <c r="D127" s="12"/>
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
-      <c r="I127" s="12"/>
-      <c r="J127" s="13"/>
+      <c r="I127" s="13"/>
+      <c r="J127" s="12"/>
       <c r="K127" s="12"/>
       <c r="L127" s="12"/>
       <c r="M127" s="12"/>
-      <c r="N127" s="12"/>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128"/>
       <c r="B128" s="12"/>
-      <c r="C128" s="13"/>
+      <c r="C128" s="12"/>
       <c r="D128" s="12"/>
       <c r="E128" s="12"/>
       <c r="F128" s="12"/>
       <c r="G128" s="12"/>
       <c r="H128" s="12"/>
-      <c r="I128" s="12"/>
-      <c r="J128" s="13"/>
+      <c r="I128" s="13"/>
+      <c r="J128" s="12"/>
       <c r="K128" s="12"/>
       <c r="L128" s="12"/>
       <c r="M128" s="12"/>
-      <c r="N128" s="12"/>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129"/>
       <c r="B129" s="12"/>
-      <c r="C129" s="13"/>
+      <c r="C129" s="12"/>
       <c r="D129" s="12"/>
       <c r="E129" s="12"/>
       <c r="F129" s="12"/>
       <c r="G129" s="12"/>
       <c r="H129" s="12"/>
-      <c r="I129" s="12"/>
-      <c r="J129" s="13"/>
+      <c r="I129" s="13"/>
+      <c r="J129" s="12"/>
       <c r="K129" s="12"/>
       <c r="L129" s="12"/>
       <c r="M129" s="12"/>
-      <c r="N129" s="12"/>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130"/>
       <c r="B130" s="12"/>
-      <c r="C130" s="13"/>
+      <c r="C130" s="12"/>
       <c r="D130" s="12"/>
       <c r="E130" s="12"/>
       <c r="F130" s="12"/>
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
-      <c r="I130" s="12"/>
-      <c r="J130" s="13"/>
+      <c r="I130" s="13"/>
+      <c r="J130" s="12"/>
       <c r="K130" s="12"/>
       <c r="L130" s="12"/>
       <c r="M130" s="12"/>
-      <c r="N130" s="12"/>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131"/>
       <c r="B131" s="12"/>
-      <c r="C131" s="13"/>
+      <c r="C131" s="12"/>
       <c r="D131" s="12"/>
       <c r="E131" s="12"/>
       <c r="F131" s="12"/>
       <c r="G131" s="12"/>
       <c r="H131" s="12"/>
-      <c r="I131" s="12"/>
-      <c r="J131" s="13"/>
+      <c r="I131" s="13"/>
+      <c r="J131" s="12"/>
       <c r="K131" s="12"/>
       <c r="L131" s="12"/>
       <c r="M131" s="12"/>
-      <c r="N131" s="12"/>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132"/>
       <c r="B132" s="12"/>
-      <c r="C132" s="13"/>
+      <c r="C132" s="12"/>
       <c r="D132" s="12"/>
       <c r="E132" s="12"/>
       <c r="F132" s="12"/>
       <c r="G132" s="12"/>
       <c r="H132" s="12"/>
-      <c r="I132" s="12"/>
-      <c r="J132" s="13"/>
+      <c r="I132" s="13"/>
+      <c r="J132" s="12"/>
       <c r="K132" s="12"/>
       <c r="L132" s="12"/>
       <c r="M132" s="12"/>
-      <c r="N132" s="12"/>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133"/>
       <c r="B133" s="12"/>
-      <c r="C133" s="13"/>
+      <c r="C133" s="12"/>
       <c r="D133" s="12"/>
       <c r="E133" s="12"/>
       <c r="F133" s="12"/>
       <c r="G133" s="12"/>
       <c r="H133" s="12"/>
-      <c r="I133" s="12"/>
-      <c r="J133" s="13"/>
+      <c r="I133" s="13"/>
+      <c r="J133" s="12"/>
       <c r="K133" s="12"/>
       <c r="L133" s="12"/>
       <c r="M133" s="12"/>
-      <c r="N133" s="12"/>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134"/>
       <c r="B134" s="12"/>
-      <c r="C134" s="13"/>
+      <c r="C134" s="12"/>
       <c r="D134" s="12"/>
       <c r="E134" s="12"/>
       <c r="F134" s="12"/>
       <c r="G134" s="12"/>
       <c r="H134" s="12"/>
-      <c r="I134" s="12"/>
-      <c r="J134" s="13"/>
+      <c r="I134" s="13"/>
+      <c r="J134" s="12"/>
       <c r="K134" s="12"/>
       <c r="L134" s="12"/>
       <c r="M134" s="12"/>
-      <c r="N134" s="12"/>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135"/>
       <c r="B135" s="12"/>
-      <c r="C135" s="13"/>
+      <c r="C135" s="12"/>
       <c r="D135" s="12"/>
       <c r="E135" s="12"/>
       <c r="F135" s="12"/>
       <c r="G135" s="12"/>
       <c r="H135" s="12"/>
-      <c r="I135" s="12"/>
-      <c r="J135" s="13"/>
+      <c r="I135" s="13"/>
+      <c r="J135" s="12"/>
       <c r="K135" s="12"/>
       <c r="L135" s="12"/>
       <c r="M135" s="12"/>
-      <c r="N135" s="12"/>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136"/>
       <c r="B136" s="12"/>
-      <c r="C136" s="13"/>
+      <c r="C136" s="12"/>
       <c r="D136" s="12"/>
       <c r="E136" s="12"/>
       <c r="F136" s="12"/>
       <c r="G136" s="12"/>
       <c r="H136" s="12"/>
-      <c r="I136" s="12"/>
-      <c r="J136" s="13"/>
+      <c r="I136" s="13"/>
+      <c r="J136" s="12"/>
       <c r="K136" s="12"/>
       <c r="L136" s="12"/>
       <c r="M136" s="12"/>
-      <c r="N136" s="12"/>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137"/>
       <c r="B137" s="12"/>
-      <c r="C137" s="13"/>
+      <c r="C137" s="12"/>
       <c r="D137" s="12"/>
       <c r="E137" s="12"/>
       <c r="F137" s="12"/>
       <c r="G137" s="12"/>
       <c r="H137" s="12"/>
-      <c r="I137" s="12"/>
-      <c r="J137" s="13"/>
+      <c r="I137" s="13"/>
+      <c r="J137" s="12"/>
       <c r="K137" s="12"/>
       <c r="L137" s="12"/>
       <c r="M137" s="12"/>
-      <c r="N137" s="12"/>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138"/>
       <c r="B138" s="12"/>
-      <c r="C138" s="13"/>
+      <c r="C138" s="12"/>
       <c r="D138" s="12"/>
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
       <c r="G138" s="12"/>
       <c r="H138" s="12"/>
-      <c r="I138" s="12"/>
-      <c r="J138" s="13"/>
+      <c r="I138" s="13"/>
+      <c r="J138" s="12"/>
       <c r="K138" s="12"/>
       <c r="L138" s="12"/>
       <c r="M138" s="12"/>
-      <c r="N138" s="12"/>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139"/>
       <c r="B139" s="12"/>
-      <c r="C139" s="13"/>
+      <c r="C139" s="12"/>
       <c r="D139" s="12"/>
       <c r="E139" s="12"/>
       <c r="F139" s="12"/>
       <c r="G139" s="12"/>
       <c r="H139" s="12"/>
-      <c r="I139" s="12"/>
-      <c r="J139" s="13"/>
+      <c r="I139" s="13"/>
+      <c r="J139" s="12"/>
       <c r="K139" s="12"/>
       <c r="L139" s="12"/>
       <c r="M139" s="12"/>
-      <c r="N139" s="12"/>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140"/>
       <c r="B140" s="12"/>
-      <c r="C140" s="13"/>
+      <c r="C140" s="12"/>
       <c r="D140" s="12"/>
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
       <c r="G140" s="12"/>
       <c r="H140" s="12"/>
-      <c r="I140" s="12"/>
-      <c r="J140" s="13"/>
+      <c r="I140" s="13"/>
+      <c r="J140" s="12"/>
       <c r="K140" s="12"/>
       <c r="L140" s="12"/>
       <c r="M140" s="12"/>
-      <c r="N140" s="12"/>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141"/>
       <c r="B141" s="12"/>
-      <c r="C141" s="13"/>
+      <c r="C141" s="12"/>
       <c r="D141" s="12"/>
       <c r="E141" s="12"/>
       <c r="F141" s="12"/>
       <c r="G141" s="12"/>
       <c r="H141" s="12"/>
-      <c r="I141" s="12"/>
-      <c r="J141" s="13"/>
+      <c r="I141" s="13"/>
+      <c r="J141" s="12"/>
       <c r="K141" s="12"/>
       <c r="L141" s="12"/>
       <c r="M141" s="12"/>
-      <c r="N141" s="12"/>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142"/>
       <c r="B142" s="12"/>
-      <c r="C142" s="13"/>
+      <c r="C142" s="12"/>
       <c r="D142" s="12"/>
       <c r="E142" s="12"/>
       <c r="F142" s="12"/>
       <c r="G142" s="12"/>
       <c r="H142" s="12"/>
-      <c r="I142" s="12"/>
-      <c r="J142" s="13"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="12"/>
       <c r="K142" s="12"/>
       <c r="L142" s="12"/>
       <c r="M142" s="12"/>
-      <c r="N142" s="12"/>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143"/>
       <c r="B143" s="12"/>
-      <c r="C143" s="13"/>
+      <c r="C143" s="12"/>
       <c r="D143" s="12"/>
       <c r="E143" s="12"/>
       <c r="F143" s="12"/>
       <c r="G143" s="12"/>
       <c r="H143" s="12"/>
-      <c r="I143" s="12"/>
-      <c r="J143" s="13"/>
+      <c r="I143" s="13"/>
+      <c r="J143" s="12"/>
       <c r="K143" s="12"/>
       <c r="L143" s="12"/>
       <c r="M143" s="12"/>
-      <c r="N143" s="12"/>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144"/>
       <c r="B144" s="12"/>
-      <c r="C144" s="13"/>
+      <c r="C144" s="12"/>
       <c r="D144" s="12"/>
       <c r="E144" s="12"/>
       <c r="F144" s="12"/>
       <c r="G144" s="12"/>
       <c r="H144" s="12"/>
-      <c r="I144" s="12"/>
-      <c r="J144" s="13"/>
+      <c r="I144" s="13"/>
+      <c r="J144" s="12"/>
       <c r="K144" s="12"/>
       <c r="L144" s="12"/>
       <c r="M144" s="12"/>
-      <c r="N144" s="12"/>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145"/>
       <c r="B145" s="12"/>
-      <c r="C145" s="13"/>
+      <c r="C145" s="12"/>
       <c r="D145" s="12"/>
       <c r="E145" s="12"/>
       <c r="F145" s="12"/>
       <c r="G145" s="12"/>
       <c r="H145" s="12"/>
-      <c r="I145" s="12"/>
-      <c r="J145" s="13"/>
+      <c r="I145" s="13"/>
+      <c r="J145" s="12"/>
       <c r="K145" s="12"/>
       <c r="L145" s="12"/>
       <c r="M145" s="12"/>
-      <c r="N145" s="12"/>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146"/>
       <c r="B146" s="12"/>
-      <c r="C146" s="13"/>
+      <c r="C146" s="12"/>
       <c r="D146" s="12"/>
       <c r="E146" s="12"/>
       <c r="F146" s="12"/>
       <c r="G146" s="12"/>
       <c r="H146" s="12"/>
-      <c r="I146" s="12"/>
-      <c r="J146" s="13"/>
+      <c r="I146" s="13"/>
+      <c r="J146" s="12"/>
       <c r="K146" s="12"/>
       <c r="L146" s="12"/>
       <c r="M146" s="12"/>
-      <c r="N146" s="12"/>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147"/>
       <c r="B147" s="12"/>
-      <c r="C147" s="13"/>
+      <c r="C147" s="12"/>
       <c r="D147" s="12"/>
       <c r="E147" s="12"/>
       <c r="F147" s="12"/>
       <c r="G147" s="12"/>
       <c r="H147" s="12"/>
-      <c r="I147" s="12"/>
-      <c r="J147" s="13"/>
+      <c r="I147" s="13"/>
+      <c r="J147" s="12"/>
       <c r="K147" s="12"/>
       <c r="L147" s="12"/>
       <c r="M147" s="12"/>
-      <c r="N147" s="12"/>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148"/>
       <c r="B148" s="12"/>
-      <c r="C148" s="13"/>
+      <c r="C148" s="12"/>
       <c r="D148" s="12"/>
       <c r="E148" s="12"/>
       <c r="F148" s="12"/>
       <c r="G148" s="12"/>
       <c r="H148" s="12"/>
-      <c r="I148" s="12"/>
-      <c r="J148" s="13"/>
+      <c r="I148" s="13"/>
+      <c r="J148" s="12"/>
       <c r="K148" s="12"/>
       <c r="L148" s="12"/>
       <c r="M148" s="12"/>
-      <c r="N148" s="12"/>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149"/>
       <c r="B149" s="12"/>
-      <c r="C149" s="13"/>
+      <c r="C149" s="12"/>
       <c r="D149" s="12"/>
       <c r="E149" s="12"/>
       <c r="F149" s="12"/>
       <c r="G149" s="12"/>
       <c r="H149" s="12"/>
-      <c r="I149" s="12"/>
-      <c r="J149" s="13"/>
+      <c r="I149" s="13"/>
+      <c r="J149" s="12"/>
       <c r="K149" s="12"/>
       <c r="L149" s="12"/>
       <c r="M149" s="12"/>
-      <c r="N149" s="12"/>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150"/>
       <c r="B150" s="12"/>
-      <c r="C150" s="13"/>
+      <c r="C150" s="12"/>
       <c r="D150" s="12"/>
       <c r="E150" s="12"/>
       <c r="F150" s="12"/>
       <c r="G150" s="12"/>
       <c r="H150" s="12"/>
-      <c r="I150" s="12"/>
-      <c r="J150" s="13"/>
+      <c r="I150" s="13"/>
+      <c r="J150" s="12"/>
       <c r="K150" s="12"/>
       <c r="L150" s="12"/>
       <c r="M150" s="12"/>
-      <c r="N150" s="12"/>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151"/>
       <c r="B151" s="12"/>
-      <c r="C151" s="13"/>
+      <c r="C151" s="12"/>
       <c r="D151" s="12"/>
       <c r="E151" s="12"/>
       <c r="F151" s="12"/>
       <c r="G151" s="12"/>
       <c r="H151" s="12"/>
-      <c r="I151" s="12"/>
-      <c r="J151" s="13"/>
+      <c r="I151" s="13"/>
+      <c r="J151" s="12"/>
       <c r="K151" s="12"/>
       <c r="L151" s="12"/>
       <c r="M151" s="12"/>
-      <c r="N151" s="12"/>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152"/>
       <c r="B152" s="12"/>
-      <c r="C152" s="13"/>
+      <c r="C152" s="12"/>
       <c r="D152" s="12"/>
       <c r="E152" s="12"/>
       <c r="F152" s="12"/>
       <c r="G152" s="12"/>
       <c r="H152" s="12"/>
-      <c r="I152" s="12"/>
-      <c r="J152" s="13"/>
+      <c r="I152" s="13"/>
+      <c r="J152" s="12"/>
       <c r="K152" s="12"/>
       <c r="L152" s="12"/>
       <c r="M152" s="12"/>
-      <c r="N152" s="12"/>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153"/>
       <c r="B153" s="12"/>
-      <c r="C153" s="13"/>
+      <c r="C153" s="12"/>
       <c r="D153" s="12"/>
       <c r="E153" s="12"/>
       <c r="F153" s="12"/>
       <c r="G153" s="12"/>
       <c r="H153" s="12"/>
-      <c r="I153" s="12"/>
-      <c r="J153" s="13"/>
+      <c r="I153" s="13"/>
+      <c r="J153" s="12"/>
       <c r="K153" s="12"/>
       <c r="L153" s="12"/>
       <c r="M153" s="12"/>
-      <c r="N153" s="12"/>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154"/>
       <c r="B154" s="12"/>
-      <c r="C154" s="13"/>
+      <c r="C154" s="12"/>
       <c r="D154" s="12"/>
       <c r="E154" s="12"/>
       <c r="F154" s="12"/>
       <c r="G154" s="12"/>
       <c r="H154" s="12"/>
-      <c r="I154" s="12"/>
-      <c r="J154" s="13"/>
+      <c r="I154" s="13"/>
+      <c r="J154" s="12"/>
       <c r="K154" s="12"/>
       <c r="L154" s="12"/>
       <c r="M154" s="12"/>
-      <c r="N154" s="12"/>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155"/>
       <c r="B155" s="12"/>
-      <c r="C155" s="13"/>
+      <c r="C155" s="12"/>
       <c r="D155" s="12"/>
       <c r="E155" s="12"/>
       <c r="F155" s="12"/>
       <c r="G155" s="12"/>
       <c r="H155" s="12"/>
-      <c r="I155" s="12"/>
-      <c r="J155" s="13"/>
+      <c r="I155" s="13"/>
+      <c r="J155" s="12"/>
       <c r="K155" s="12"/>
       <c r="L155" s="12"/>
       <c r="M155" s="12"/>
-      <c r="N155" s="12"/>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156"/>
       <c r="B156" s="12"/>
-      <c r="C156" s="13"/>
+      <c r="C156" s="12"/>
       <c r="D156" s="12"/>
       <c r="E156" s="12"/>
       <c r="F156" s="12"/>
       <c r="G156" s="12"/>
       <c r="H156" s="12"/>
-      <c r="I156" s="12"/>
-      <c r="J156" s="13"/>
+      <c r="I156" s="13"/>
+      <c r="J156" s="12"/>
       <c r="K156" s="12"/>
       <c r="L156" s="12"/>
       <c r="M156" s="12"/>
-      <c r="N156" s="12"/>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157"/>
       <c r="B157" s="12"/>
-      <c r="C157" s="13"/>
+      <c r="C157" s="12"/>
       <c r="D157" s="12"/>
       <c r="E157" s="12"/>
       <c r="F157" s="12"/>
       <c r="G157" s="12"/>
       <c r="H157" s="12"/>
-      <c r="I157" s="12"/>
-      <c r="J157" s="13"/>
+      <c r="I157" s="13"/>
+      <c r="J157" s="12"/>
       <c r="K157" s="12"/>
       <c r="L157" s="12"/>
       <c r="M157" s="12"/>
-      <c r="N157" s="12"/>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158"/>
       <c r="B158" s="12"/>
-      <c r="C158" s="13"/>
+      <c r="C158" s="12"/>
       <c r="D158" s="12"/>
       <c r="E158" s="12"/>
       <c r="F158" s="12"/>
       <c r="G158" s="12"/>
       <c r="H158" s="12"/>
-      <c r="I158" s="12"/>
-      <c r="J158" s="13"/>
+      <c r="I158" s="13"/>
+      <c r="J158" s="12"/>
       <c r="K158" s="12"/>
       <c r="L158" s="12"/>
       <c r="M158" s="12"/>
-      <c r="N158" s="12"/>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159"/>
       <c r="B159" s="12"/>
-      <c r="C159" s="13"/>
+      <c r="C159" s="12"/>
       <c r="D159" s="12"/>
       <c r="E159" s="12"/>
       <c r="F159" s="12"/>
       <c r="G159" s="12"/>
       <c r="H159" s="12"/>
-      <c r="I159" s="12"/>
-      <c r="J159" s="13"/>
+      <c r="I159" s="13"/>
+      <c r="J159" s="12"/>
       <c r="K159" s="12"/>
       <c r="L159" s="12"/>
       <c r="M159" s="12"/>
-      <c r="N159" s="12"/>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160"/>
       <c r="B160" s="12"/>
-      <c r="C160" s="13"/>
+      <c r="C160" s="12"/>
       <c r="D160" s="12"/>
       <c r="E160" s="12"/>
       <c r="F160" s="12"/>
       <c r="G160" s="12"/>
       <c r="H160" s="12"/>
-      <c r="I160" s="12"/>
-      <c r="J160" s="13"/>
+      <c r="I160" s="13"/>
+      <c r="J160" s="12"/>
       <c r="K160" s="12"/>
       <c r="L160" s="12"/>
       <c r="M160" s="12"/>
-      <c r="N160" s="12"/>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161"/>
       <c r="B161" s="12"/>
-      <c r="C161" s="13"/>
+      <c r="C161" s="12"/>
       <c r="D161" s="12"/>
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
       <c r="G161" s="12"/>
       <c r="H161" s="12"/>
-      <c r="I161" s="12"/>
-      <c r="J161" s="13"/>
+      <c r="I161" s="13"/>
+      <c r="J161" s="12"/>
       <c r="K161" s="12"/>
       <c r="L161" s="12"/>
       <c r="M161" s="12"/>
-      <c r="N161" s="12"/>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162"/>
       <c r="B162" s="12"/>
-      <c r="C162" s="13"/>
+      <c r="C162" s="12"/>
       <c r="D162" s="12"/>
       <c r="E162" s="12"/>
       <c r="F162" s="12"/>
       <c r="G162" s="12"/>
       <c r="H162" s="12"/>
-      <c r="I162" s="12"/>
-      <c r="J162" s="13"/>
+      <c r="I162" s="13"/>
+      <c r="J162" s="12"/>
       <c r="K162" s="12"/>
       <c r="L162" s="12"/>
       <c r="M162" s="12"/>
-      <c r="N162" s="12"/>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163"/>
       <c r="B163" s="12"/>
-      <c r="C163" s="13"/>
+      <c r="C163" s="12"/>
       <c r="D163" s="12"/>
       <c r="E163" s="12"/>
       <c r="F163" s="12"/>
       <c r="G163" s="12"/>
       <c r="H163" s="12"/>
-      <c r="I163" s="12"/>
-      <c r="J163" s="13"/>
+      <c r="I163" s="13"/>
+      <c r="J163" s="12"/>
       <c r="K163" s="12"/>
       <c r="L163" s="12"/>
       <c r="M163" s="12"/>
-      <c r="N163" s="12"/>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164"/>
       <c r="B164" s="12"/>
-      <c r="C164" s="13"/>
+      <c r="C164" s="12"/>
       <c r="D164" s="12"/>
       <c r="E164" s="12"/>
       <c r="F164" s="12"/>
       <c r="G164" s="12"/>
       <c r="H164" s="12"/>
-      <c r="I164" s="12"/>
-      <c r="J164" s="13"/>
+      <c r="I164" s="13"/>
+      <c r="J164" s="12"/>
       <c r="K164" s="12"/>
       <c r="L164" s="12"/>
       <c r="M164" s="12"/>
-      <c r="N164" s="12"/>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165"/>
       <c r="B165" s="12"/>
-      <c r="C165" s="13"/>
+      <c r="C165" s="12"/>
       <c r="D165" s="12"/>
       <c r="E165" s="12"/>
       <c r="F165" s="12"/>
       <c r="G165" s="12"/>
       <c r="H165" s="12"/>
-      <c r="I165" s="12"/>
-      <c r="J165" s="13"/>
+      <c r="I165" s="13"/>
+      <c r="J165" s="12"/>
       <c r="K165" s="12"/>
       <c r="L165" s="12"/>
       <c r="M165" s="12"/>
-      <c r="N165" s="12"/>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166"/>
       <c r="B166" s="12"/>
-      <c r="C166" s="13"/>
+      <c r="C166" s="12"/>
       <c r="D166" s="12"/>
       <c r="E166" s="12"/>
       <c r="F166" s="12"/>
       <c r="G166" s="12"/>
       <c r="H166" s="12"/>
-      <c r="I166" s="12"/>
-      <c r="J166" s="13"/>
+      <c r="I166" s="13"/>
+      <c r="J166" s="12"/>
       <c r="K166" s="12"/>
       <c r="L166" s="12"/>
       <c r="M166" s="12"/>
-      <c r="N166" s="12"/>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167"/>
       <c r="B167" s="12"/>
-      <c r="C167" s="13"/>
+      <c r="C167" s="12"/>
       <c r="D167" s="12"/>
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
-      <c r="I167" s="12"/>
-      <c r="J167" s="13"/>
+      <c r="I167" s="13"/>
+      <c r="J167" s="12"/>
       <c r="K167" s="12"/>
       <c r="L167" s="12"/>
       <c r="M167" s="12"/>
-      <c r="N167" s="12"/>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168"/>
       <c r="B168" s="12"/>
-      <c r="C168" s="13"/>
+      <c r="C168" s="12"/>
       <c r="D168" s="12"/>
       <c r="E168" s="12"/>
       <c r="F168" s="12"/>
       <c r="G168" s="12"/>
       <c r="H168" s="12"/>
-      <c r="I168" s="12"/>
-      <c r="J168" s="13"/>
+      <c r="I168" s="13"/>
+      <c r="J168" s="12"/>
       <c r="K168" s="12"/>
       <c r="L168" s="12"/>
       <c r="M168" s="12"/>
-      <c r="N168" s="12"/>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169"/>
       <c r="B169" s="12"/>
-      <c r="C169" s="13"/>
+      <c r="C169" s="12"/>
       <c r="D169" s="12"/>
       <c r="E169" s="12"/>
       <c r="F169" s="12"/>
       <c r="G169" s="12"/>
       <c r="H169" s="12"/>
-      <c r="I169" s="12"/>
-      <c r="J169" s="13"/>
+      <c r="I169" s="13"/>
+      <c r="J169" s="12"/>
       <c r="K169" s="12"/>
       <c r="L169" s="12"/>
       <c r="M169" s="12"/>
-      <c r="N169" s="12"/>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170"/>
       <c r="B170" s="12"/>
-      <c r="C170" s="13"/>
+      <c r="C170" s="12"/>
       <c r="D170" s="12"/>
       <c r="E170" s="12"/>
       <c r="F170" s="12"/>
       <c r="G170" s="12"/>
       <c r="H170" s="12"/>
-      <c r="I170" s="12"/>
-      <c r="J170" s="13"/>
+      <c r="I170" s="13"/>
+      <c r="J170" s="12"/>
       <c r="K170" s="12"/>
       <c r="L170" s="12"/>
       <c r="M170" s="12"/>
-      <c r="N170" s="12"/>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171"/>
       <c r="B171" s="12"/>
-      <c r="C171" s="13"/>
+      <c r="C171" s="12"/>
       <c r="D171" s="12"/>
       <c r="E171" s="12"/>
       <c r="F171" s="12"/>
       <c r="G171" s="12"/>
       <c r="H171" s="12"/>
-      <c r="I171" s="12"/>
-      <c r="J171" s="13"/>
+      <c r="I171" s="13"/>
+      <c r="J171" s="12"/>
       <c r="K171" s="12"/>
       <c r="L171" s="12"/>
       <c r="M171" s="12"/>
-      <c r="N171" s="12"/>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172"/>
       <c r="B172" s="12"/>
-      <c r="C172" s="13"/>
+      <c r="C172" s="12"/>
       <c r="D172" s="12"/>
       <c r="E172" s="12"/>
       <c r="F172" s="12"/>
       <c r="G172" s="12"/>
       <c r="H172" s="12"/>
-      <c r="I172" s="12"/>
-      <c r="J172" s="13"/>
+      <c r="I172" s="13"/>
+      <c r="J172" s="12"/>
       <c r="K172" s="12"/>
       <c r="L172" s="12"/>
       <c r="M172" s="12"/>
-      <c r="N172" s="12"/>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173"/>
       <c r="B173" s="12"/>
-      <c r="C173" s="13"/>
+      <c r="C173" s="12"/>
       <c r="D173" s="12"/>
       <c r="E173" s="12"/>
       <c r="F173" s="12"/>
       <c r="G173" s="12"/>
       <c r="H173" s="12"/>
-      <c r="I173" s="12"/>
-      <c r="J173" s="13"/>
+      <c r="I173" s="13"/>
+      <c r="J173" s="12"/>
       <c r="K173" s="12"/>
       <c r="L173" s="12"/>
       <c r="M173" s="12"/>
-      <c r="N173" s="12"/>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174"/>
       <c r="B174" s="12"/>
-      <c r="C174" s="13"/>
+      <c r="C174" s="12"/>
       <c r="D174" s="12"/>
       <c r="E174" s="12"/>
       <c r="F174" s="12"/>
       <c r="G174" s="12"/>
       <c r="H174" s="12"/>
-      <c r="I174" s="12"/>
-      <c r="J174" s="13"/>
+      <c r="I174" s="13"/>
+      <c r="J174" s="12"/>
       <c r="K174" s="12"/>
       <c r="L174" s="12"/>
       <c r="M174" s="12"/>
-      <c r="N174" s="12"/>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175"/>
       <c r="B175" s="12"/>
-      <c r="C175" s="13"/>
+      <c r="C175" s="12"/>
       <c r="D175" s="12"/>
       <c r="E175" s="12"/>
       <c r="F175" s="12"/>
       <c r="G175" s="12"/>
       <c r="H175" s="12"/>
-      <c r="I175" s="12"/>
-      <c r="J175" s="13"/>
+      <c r="I175" s="13"/>
+      <c r="J175" s="12"/>
       <c r="K175" s="12"/>
       <c r="L175" s="12"/>
       <c r="M175" s="12"/>
-      <c r="N175" s="12"/>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176"/>
       <c r="B176" s="12"/>
-      <c r="C176" s="13"/>
+      <c r="C176" s="12"/>
       <c r="D176" s="12"/>
       <c r="E176" s="12"/>
       <c r="F176" s="12"/>
       <c r="G176" s="12"/>
       <c r="H176" s="12"/>
-      <c r="I176" s="12"/>
-      <c r="J176" s="13"/>
+      <c r="I176" s="13"/>
+      <c r="J176" s="12"/>
       <c r="K176" s="12"/>
       <c r="L176" s="12"/>
       <c r="M176" s="12"/>
-      <c r="N176" s="12"/>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177"/>
       <c r="B177" s="12"/>
-      <c r="C177" s="13"/>
+      <c r="C177" s="12"/>
       <c r="D177" s="12"/>
       <c r="E177" s="12"/>
       <c r="F177" s="12"/>
       <c r="G177" s="12"/>
       <c r="H177" s="12"/>
-      <c r="I177" s="12"/>
-      <c r="J177" s="13"/>
+      <c r="I177" s="13"/>
+      <c r="J177" s="12"/>
       <c r="K177" s="12"/>
       <c r="L177" s="12"/>
       <c r="M177" s="12"/>
-      <c r="N177" s="12"/>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178"/>
       <c r="B178" s="12"/>
-      <c r="C178" s="13"/>
+      <c r="C178" s="12"/>
       <c r="D178" s="12"/>
       <c r="E178" s="12"/>
       <c r="F178" s="12"/>
       <c r="G178" s="12"/>
       <c r="H178" s="12"/>
-      <c r="I178" s="12"/>
-      <c r="J178" s="13"/>
+      <c r="I178" s="13"/>
+      <c r="J178" s="12"/>
       <c r="K178" s="12"/>
       <c r="L178" s="12"/>
       <c r="M178" s="12"/>
-      <c r="N178" s="12"/>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179"/>
       <c r="B179" s="12"/>
-      <c r="C179" s="13"/>
+      <c r="C179" s="12"/>
       <c r="D179" s="12"/>
       <c r="E179" s="12"/>
       <c r="F179" s="12"/>
       <c r="G179" s="12"/>
       <c r="H179" s="12"/>
-      <c r="I179" s="12"/>
-      <c r="J179" s="13"/>
+      <c r="I179" s="13"/>
+      <c r="J179" s="12"/>
       <c r="K179" s="12"/>
       <c r="L179" s="12"/>
       <c r="M179" s="12"/>
-      <c r="N179" s="12"/>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180"/>
       <c r="B180" s="12"/>
-      <c r="C180" s="13"/>
+      <c r="C180" s="12"/>
       <c r="D180" s="12"/>
       <c r="E180" s="12"/>
       <c r="F180" s="12"/>
       <c r="G180" s="12"/>
       <c r="H180" s="12"/>
-      <c r="I180" s="12"/>
-      <c r="J180" s="13"/>
+      <c r="I180" s="13"/>
+      <c r="J180" s="12"/>
       <c r="K180" s="12"/>
       <c r="L180" s="12"/>
       <c r="M180" s="12"/>
-      <c r="N180" s="12"/>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181"/>
       <c r="B181" s="12"/>
-      <c r="C181" s="13"/>
+      <c r="C181" s="12"/>
       <c r="D181" s="12"/>
       <c r="E181" s="12"/>
       <c r="F181" s="12"/>
       <c r="G181" s="12"/>
       <c r="H181" s="12"/>
-      <c r="I181" s="12"/>
-      <c r="J181" s="13"/>
+      <c r="I181" s="13"/>
+      <c r="J181" s="12"/>
       <c r="K181" s="12"/>
       <c r="L181" s="12"/>
       <c r="M181" s="12"/>
-      <c r="N181" s="12"/>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182"/>
       <c r="B182" s="12"/>
-      <c r="C182" s="13"/>
+      <c r="C182" s="12"/>
       <c r="D182" s="12"/>
       <c r="E182" s="12"/>
       <c r="F182" s="12"/>
       <c r="G182" s="12"/>
       <c r="H182" s="12"/>
-      <c r="I182" s="12"/>
-      <c r="J182" s="13"/>
+      <c r="I182" s="13"/>
+      <c r="J182" s="12"/>
       <c r="K182" s="12"/>
       <c r="L182" s="12"/>
       <c r="M182" s="12"/>
-      <c r="N182" s="12"/>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183"/>
       <c r="B183" s="12"/>
-      <c r="C183" s="13"/>
+      <c r="C183" s="12"/>
       <c r="D183" s="12"/>
       <c r="E183" s="12"/>
       <c r="F183" s="12"/>
       <c r="G183" s="12"/>
       <c r="H183" s="12"/>
-      <c r="I183" s="12"/>
-      <c r="J183" s="13"/>
+      <c r="I183" s="13"/>
+      <c r="J183" s="12"/>
       <c r="K183" s="12"/>
       <c r="L183" s="12"/>
       <c r="M183" s="12"/>
-      <c r="N183" s="12"/>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184"/>
       <c r="B184" s="12"/>
-      <c r="C184" s="13"/>
+      <c r="C184" s="12"/>
       <c r="D184" s="12"/>
       <c r="E184" s="12"/>
       <c r="F184" s="12"/>
       <c r="G184" s="12"/>
       <c r="H184" s="12"/>
-      <c r="I184" s="12"/>
-      <c r="J184" s="13"/>
+      <c r="I184" s="13"/>
+      <c r="J184" s="12"/>
       <c r="K184" s="12"/>
       <c r="L184" s="12"/>
       <c r="M184" s="12"/>
-      <c r="N184" s="12"/>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185"/>
       <c r="B185" s="12"/>
-      <c r="C185" s="13"/>
+      <c r="C185" s="12"/>
       <c r="D185" s="12"/>
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
       <c r="G185" s="12"/>
       <c r="H185" s="12"/>
-      <c r="I185" s="12"/>
-      <c r="J185" s="13"/>
+      <c r="I185" s="13"/>
+      <c r="J185" s="12"/>
       <c r="K185" s="12"/>
       <c r="L185" s="12"/>
       <c r="M185" s="12"/>
-      <c r="N185" s="12"/>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186"/>
       <c r="B186" s="12"/>
-      <c r="C186" s="13"/>
+      <c r="C186" s="12"/>
       <c r="D186" s="12"/>
       <c r="E186" s="12"/>
       <c r="F186" s="12"/>
       <c r="G186" s="12"/>
       <c r="H186" s="12"/>
-      <c r="I186" s="12"/>
-      <c r="J186" s="13"/>
+      <c r="I186" s="13"/>
+      <c r="J186" s="12"/>
       <c r="K186" s="12"/>
       <c r="L186" s="12"/>
       <c r="M186" s="12"/>
-      <c r="N186" s="12"/>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187"/>
       <c r="B187" s="12"/>
-      <c r="C187" s="13"/>
+      <c r="C187" s="12"/>
       <c r="D187" s="12"/>
       <c r="E187" s="12"/>
       <c r="F187" s="12"/>
       <c r="G187" s="12"/>
       <c r="H187" s="12"/>
-      <c r="I187" s="12"/>
-      <c r="J187" s="13"/>
+      <c r="I187" s="13"/>
+      <c r="J187" s="12"/>
       <c r="K187" s="12"/>
       <c r="L187" s="12"/>
       <c r="M187" s="12"/>
-      <c r="N187" s="12"/>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188"/>
       <c r="B188" s="12"/>
-      <c r="C188" s="13"/>
+      <c r="C188" s="12"/>
       <c r="D188" s="12"/>
       <c r="E188" s="12"/>
       <c r="F188" s="12"/>
       <c r="G188" s="12"/>
       <c r="H188" s="12"/>
-      <c r="I188" s="12"/>
-      <c r="J188" s="13"/>
+      <c r="I188" s="13"/>
+      <c r="J188" s="12"/>
       <c r="K188" s="12"/>
       <c r="L188" s="12"/>
       <c r="M188" s="12"/>
-      <c r="N188" s="12"/>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189"/>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190"/>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191"/>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
@@ -52959,26 +52731,26 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1 I189:I1021" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1 H189:H1021" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>"natural,whole,interger,real"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{483D7C4D-3CB6-404A-B9C1-693F9BA7B223}">
-      <formula1>M2</formula1>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{483D7C4D-3CB6-404A-B9C1-693F9BA7B223}">
+      <formula1>L2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I188" xr:uid="{80B4E72A-B887-DF48-89F3-3DAE24F60A4C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H188" xr:uid="{80B4E72A-B887-DF48-89F3-3DAE24F60A4C}">
       <formula1>"whole, real, integer, natural"</formula1>
     </dataValidation>
   </dataValidations>
@@ -53024,7 +52796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
@@ -53050,7 +52822,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -53058,76 +52830,76 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>140</v>
+      <c r="E4" t="s">
+        <v>75</v>
       </c>
-      <c r="D3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>74</v>
       </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
       <c r="C5" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -53171,10 +52943,10 @@
     </row>
     <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -53207,27 +52979,27 @@
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>85</v>
-      </c>
-    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -53271,7 +53043,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -53329,25 +53101,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
-        <v>69</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -53404,14 +53176,14 @@
     </row>
     <row r="2" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -53451,10 +53223,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -53518,7 +53290,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1">
         <v>-122.448217</v>

</xml_diff>